<commit_message>
se finaliza proceso RPA transacciones MB52 ME21N VL10B VL02N MIGO y IQ09
</commit_message>
<xml_diff>
--- a/Resources/imeis_material.xlsx
+++ b/Resources/imeis_material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyectos-vc\AutomationSAP\SAP\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1CD6E53-9692-4ABD-8C0B-53B75A856BAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6FD11D-1788-42F0-90C4-81CEF9C8BBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{460F3357-E042-4658-9DF9-BFFD146C6658}"/>
   </bookViews>
@@ -36,12 +36,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Imeis</t>
   </si>
   <si>
-    <t>355400570292586</t>
+    <t>863268050609451</t>
+  </si>
+  <si>
+    <t>863268050609683</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A6A73E-1F70-4536-90F5-8E39C1519935}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,6 +419,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
style: :memo: ajustes identado transaccion me21n y archivo excel
</commit_message>
<xml_diff>
--- a/Resources/imeis_material.xlsx
+++ b/Resources/imeis_material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyectos-vc\AutomationSAP\SAP\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6FD11D-1788-42F0-90C4-81CEF9C8BBB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A042DFAF-1549-431C-8FCC-D193615B3E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{460F3357-E042-4658-9DF9-BFFD146C6658}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,13 +59,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,9 +94,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,8 +424,8 @@
     <col min="2" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -426,5 +441,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: :bug: se realizan ajustes en el documento excel y correcion codigo lectura excel
</commit_message>
<xml_diff>
--- a/Resources/imeis_material.xlsx
+++ b/Resources/imeis_material.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyectos-vc\AutomationSAP\SAP\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A042DFAF-1549-431C-8FCC-D193615B3E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{515AEA02-7F7F-4C3F-8A53-D2CBD5B855BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{460F3357-E042-4658-9DF9-BFFD146C6658}"/>
   </bookViews>
@@ -35,23 +35,56 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>JAIME ANDRES PINILLA BARRERA</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{5F7D524C-BE0A-41D2-840B-AF492353A3CF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nota:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> El ingreso de los Imeis deben de ser existentes y que correspondan al mismo material.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Imeis</t>
+    <t>863268050609683</t>
+  </si>
+  <si>
+    <t>Imeis del material</t>
   </si>
   <si>
     <t>863268050609451</t>
-  </si>
-  <si>
-    <t>863268050609683</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,11 +94,24 @@
     </font>
     <font>
       <b/>
-      <sz val="14"/>
-      <color theme="1"/>
+      <sz val="12"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -77,7 +123,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -94,8 +140,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -113,6 +162,199 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1619250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>561975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E593103-1218-41EA-25C4-BA6D654B7529}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="38100" y="171450"/>
+          <a:ext cx="1581150" cy="390525"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1000125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1200150</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1285875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{921393AC-5BBB-29A4-CA86-EE05FAFE1C78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="952500" y="1000125"/>
+          <a:ext cx="247650" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1304925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>933450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>2914650</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>1352550</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CuadroTexto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E83BA38-1019-C260-7006-D6DE274C2144}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1304925" y="933450"/>
+          <a:ext cx="1609725" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-CO" sz="1800" b="0"/>
+            <a:t>Entrada Imeis </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -411,26 +653,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A6A73E-1F70-4536-90F5-8E39C1519935}">
-  <dimension ref="A1:A3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A6A73E-1F70-4536-90F5-8E39C1519935}">
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="62.140625" style="1" customWidth="1"/>
+    <col min="2" max="7" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.42578125" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
+    <row r="1" spans="1:1" s="2" customFormat="1" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:1" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -439,8 +680,16 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="qDW3rs/08cCZp/RWHnizcoGfFOw/klTJr4GUrP6PvLpDEP1iifnxSou4jTtQgXdnWFNDqqj7ZDEpXP0s5zdd1w==" saltValue="q6SGJKOTQ40IOpqSIQ6ACw==" spinCount="100000" sheet="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>